<commit_message>
Get sample size without males but with sibs
</commit_message>
<xml_diff>
--- a/misc_info/GAARD_sample_sets.xlsx
+++ b/misc_info/GAARD_sample_sets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t xml:space="preserve">Location (Country)</t>
   </si>
@@ -40,6 +40,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Final N 
 Dead / alive</t>
@@ -80,7 +81,7 @@
     <t xml:space="preserve">Delta</t>
   </si>
   <si>
-    <t xml:space="preserve">42 / 48</t>
+    <t xml:space="preserve">40 / 48</t>
   </si>
   <si>
     <t xml:space="preserve">34 / 45</t>
@@ -104,34 +105,37 @@
     <t xml:space="preserve">Korle-Bu (Ghana)</t>
   </si>
   <si>
+    <t xml:space="preserve">55 / 62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 / 57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88 / 61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83 / 59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madina (Ghana)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 / 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 / 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 / 79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37 / 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obuasi (Ghana)</t>
+  </si>
+  <si>
     <t xml:space="preserve">56 / 62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48 / 57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89 / 61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83 / 59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madina (Ghana)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33 / 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 / 38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48 / 79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37 / 64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Obuasi (Ghana)</t>
   </si>
   <si>
     <t xml:space="preserve">50 / 54</t>
@@ -155,6 +159,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -183,6 +188,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -371,10 +377,10 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="12.87"/>
@@ -544,10 +550,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -561,10 +567,10 @@
         <v>12</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>